<commit_message>
data: add comparison information for more programs
</commit_message>
<xml_diff>
--- a/OpenMP_Comparisons.xlsx
+++ b/OpenMP_Comparisons.xlsx
@@ -5,30 +5,43 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidhish17\Desktop\PL\Project\Parallel-Programming-Constructs\PyOMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidhish17\Desktop\PL\Project\Parallel-Programming-Constructs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC50078-ACF8-4C73-828A-DAB03E82E4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1AAF33-F0A2-4C8C-9E68-6F3E7936812A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Averages" sheetId="1" r:id="rId1"/>
-    <sheet name="Running Sum C++" sheetId="2" r:id="rId2"/>
-    <sheet name="MatMul C++" sheetId="3" r:id="rId3"/>
-    <sheet name="Dot Product C++" sheetId="4" r:id="rId4"/>
+    <sheet name="Information" sheetId="8" r:id="rId1"/>
+    <sheet name="Averages" sheetId="1" r:id="rId2"/>
+    <sheet name="Pi Computation C++" sheetId="7" r:id="rId3"/>
+    <sheet name="Running Sum C++" sheetId="2" r:id="rId4"/>
+    <sheet name="Matrix Multiplication C++" sheetId="3" r:id="rId5"/>
+    <sheet name="Dot Product C++" sheetId="4" r:id="rId6"/>
+    <sheet name="Count Primes C++" sheetId="5" r:id="rId7"/>
+    <sheet name="Merge Sort C++" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913" fullPrecision="0"/>
+  <calcPr calcId="191029" fullPrecision="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Program</t>
   </si>
@@ -66,26 +79,44 @@
     <t>Parallel (4 threads)</t>
   </si>
   <si>
-    <t>N: 10^8</t>
-  </si>
-  <si>
-    <t>Time in seconds</t>
-  </si>
-  <si>
-    <t>1000 x 1000 matrices were used</t>
-  </si>
-  <si>
-    <t>N = 10^7</t>
-  </si>
-  <si>
-    <t>Time in milliseconds</t>
+    <t>Parallel (16 threads)</t>
+  </si>
+  <si>
+    <t>Merge Sort</t>
+  </si>
+  <si>
+    <t>Running Sum</t>
+  </si>
+  <si>
+    <t>Additional Notes</t>
+  </si>
+  <si>
+    <t>The value of time is in seconds for all programs.</t>
+  </si>
+  <si>
+    <t>Compute product of two 1000 x 1000 matrices</t>
+  </si>
+  <si>
+    <t>Compute dot product of two 10,000,000 dimensional vectors</t>
+  </si>
+  <si>
+    <t>Definite integral method used, steps = 100,000,000</t>
+  </si>
+  <si>
+    <t>Copmute sum from 1 to 100,000,000</t>
+  </si>
+  <si>
+    <t>Primes are counted from 1 to 500,000</t>
+  </si>
+  <si>
+    <t>An array with 100,000,000 elements is sorted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,13 +124,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -114,8 +159,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,11 +441,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4316CE6-39B2-44DD-8FD3-04F419982031}">
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,17 +587,176 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02508278-E363-4327-8C60-69A0E62B51F4}">
-  <dimension ref="A1:E16"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625CEBF0-B641-439B-B080-CB4876D8D045}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0.41121000000000002</v>
+      </c>
+      <c r="B2">
+        <v>5.7464000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.42094300000000001</v>
+      </c>
+      <c r="B3">
+        <v>6.0519000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.41970600000000002</v>
+      </c>
+      <c r="B4">
+        <v>6.7448999999999995E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.42357</v>
+      </c>
+      <c r="B5">
+        <v>5.5787999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.41464400000000001</v>
+      </c>
+      <c r="B6">
+        <v>7.9546000000000006E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.41665400000000002</v>
+      </c>
+      <c r="B7">
+        <v>6.1622999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.412854</v>
+      </c>
+      <c r="B8">
+        <v>6.2451E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.41177200000000003</v>
+      </c>
+      <c r="B9">
+        <v>6.2102999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.41416900000000001</v>
+      </c>
+      <c r="B10">
+        <v>5.2070999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.41565400000000002</v>
+      </c>
+      <c r="B11">
+        <v>6.3840999999999995E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.420653</v>
+      </c>
+      <c r="B12">
+        <v>5.9910999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0.38577400000000001</v>
+      </c>
+      <c r="B13">
+        <v>6.7740999999999996E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0.42255500000000001</v>
+      </c>
+      <c r="B14">
+        <v>6.1046999999999997E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0.42057499999999998</v>
+      </c>
+      <c r="B15">
+        <v>5.5365999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0.38974500000000001</v>
+      </c>
+      <c r="B16">
+        <v>5.6604000000000002E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02508278-E363-4327-8C60-69A0E62B51F4}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,21 +765,15 @@
     <col min="5" max="5" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.10929999999999999</v>
       </c>
@@ -492,7 +781,7 @@
         <v>2.4674999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.11129600000000001</v>
       </c>
@@ -500,7 +789,7 @@
         <v>2.8048E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.108654</v>
       </c>
@@ -508,7 +797,7 @@
         <v>3.841E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.106431</v>
       </c>
@@ -516,7 +805,7 @@
         <v>2.1033E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.10770200000000001</v>
       </c>
@@ -524,7 +813,7 @@
         <v>2.4388E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.103633</v>
       </c>
@@ -532,7 +821,7 @@
         <v>2.0934999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.103937</v>
       </c>
@@ -540,7 +829,7 @@
         <v>2.1565999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.108137</v>
       </c>
@@ -548,7 +837,7 @@
         <v>2.7966000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.110272</v>
       </c>
@@ -556,7 +845,7 @@
         <v>2.2501E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.103302</v>
       </c>
@@ -564,7 +853,7 @@
         <v>4.0382000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.10395500000000001</v>
       </c>
@@ -572,7 +861,7 @@
         <v>2.8358999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0.10953</v>
       </c>
@@ -580,7 +869,7 @@
         <v>2.6498000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0.10675999999999999</v>
       </c>
@@ -588,7 +877,7 @@
         <v>2.1087999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0.103185</v>
       </c>
@@ -596,7 +885,7 @@
         <v>2.2419999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0.10272199999999999</v>
       </c>
@@ -609,12 +898,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7270F145-8BEB-4A03-ABA7-5F181258B856}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,138 +912,132 @@
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>5956</v>
+        <v>5.9560000000000004</v>
       </c>
       <c r="B2">
-        <v>2142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.1419999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>6029</v>
+        <v>6.0289999999999999</v>
       </c>
       <c r="B3">
-        <v>2052</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.052</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>5978</v>
+        <v>5.9779999999999998</v>
       </c>
       <c r="B4">
-        <v>2205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.2050000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>5923</v>
+        <v>5.923</v>
       </c>
       <c r="B5">
-        <v>2153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5982</v>
+        <v>5.9820000000000002</v>
       </c>
       <c r="B6">
-        <v>2248</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.2480000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5919</v>
+        <v>5.9189999999999996</v>
       </c>
       <c r="B7">
-        <v>2213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.2130000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>5997</v>
+        <v>5.9969999999999999</v>
       </c>
       <c r="B8">
-        <v>2097</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.097</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>5731</v>
+        <v>5.7309999999999999</v>
       </c>
       <c r="B9">
-        <v>2045</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.0449999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>5939</v>
+        <v>5.9390000000000001</v>
       </c>
       <c r="B10">
-        <v>2057</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.0569999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>5870</v>
+        <v>5.87</v>
       </c>
       <c r="B11">
-        <v>2234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>6092</v>
+        <v>6.0919999999999996</v>
       </c>
       <c r="B12">
-        <v>1996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>5833</v>
+        <v>5.8330000000000002</v>
       </c>
       <c r="B13">
-        <v>2342</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.3420000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>5874</v>
+        <v>5.8739999999999997</v>
       </c>
       <c r="B14">
-        <v>2101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>6010</v>
+        <v>6.01</v>
       </c>
       <c r="B15">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.3860000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>6010</v>
+        <v>6.01</v>
       </c>
       <c r="B16">
-        <v>2334</v>
+        <v>2.3340000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -762,12 +1045,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC9AE9B-1012-4872-BF7E-C5995415CA8D}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,18 +1059,15 @@
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4.3516399999999997E-2</v>
       </c>
@@ -795,7 +1075,7 @@
         <v>1.25475E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4.4568900000000002E-2</v>
       </c>
@@ -803,7 +1083,7 @@
         <v>1.39922E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4.2894000000000002E-2</v>
       </c>
@@ -811,7 +1091,7 @@
         <v>1.45378E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4.2875799999999999E-2</v>
       </c>
@@ -819,7 +1099,7 @@
         <v>1.4550499999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4.3184899999999998E-2</v>
       </c>
@@ -827,7 +1107,7 @@
         <v>1.27452E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4.4534900000000002E-2</v>
       </c>
@@ -835,7 +1115,7 @@
         <v>1.3297399999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4.4072199999999999E-2</v>
       </c>
@@ -843,7 +1123,7 @@
         <v>1.2121699999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4.48087E-2</v>
       </c>
@@ -851,7 +1131,7 @@
         <v>1.3280800000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4.7559299999999999E-2</v>
       </c>
@@ -859,7 +1139,7 @@
         <v>1.34824E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4.2725699999999998E-2</v>
       </c>
@@ -867,7 +1147,7 @@
         <v>1.33697E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4.30829E-2</v>
       </c>
@@ -875,7 +1155,7 @@
         <v>1.3571099999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4.2482800000000001E-2</v>
       </c>
@@ -883,7 +1163,7 @@
         <v>1.3606E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4.4585100000000003E-2</v>
       </c>
@@ -891,7 +1171,7 @@
         <v>1.2704399999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4.2559699999999999E-2</v>
       </c>
@@ -899,12 +1179,408 @@
         <v>1.3818499999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4.3664000000000001E-2</v>
       </c>
       <c r="B16">
         <v>1.28437E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD111DFE-1B34-4E4C-BBC5-EA342300D4FA}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="33.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>15.2575</v>
+      </c>
+      <c r="B2">
+        <v>2.8876400000000002</v>
+      </c>
+      <c r="C2">
+        <v>8.08901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>15.313700000000001</v>
+      </c>
+      <c r="B3">
+        <v>2.7796599999999998</v>
+      </c>
+      <c r="C3">
+        <v>8.2573399999999992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>15.3512</v>
+      </c>
+      <c r="B4">
+        <v>2.7237100000000001</v>
+      </c>
+      <c r="C4">
+        <v>8.1074800000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>15.331</v>
+      </c>
+      <c r="B5">
+        <v>2.8534700000000002</v>
+      </c>
+      <c r="C5">
+        <v>8.3206299999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>15.358700000000001</v>
+      </c>
+      <c r="B6">
+        <v>2.77054</v>
+      </c>
+      <c r="C6">
+        <v>8.2640899999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>15.4488</v>
+      </c>
+      <c r="B7">
+        <v>2.7242799999999998</v>
+      </c>
+      <c r="C7">
+        <v>8.4612099999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>15.520300000000001</v>
+      </c>
+      <c r="B8">
+        <v>2.7445400000000002</v>
+      </c>
+      <c r="C8">
+        <v>8.1501000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>15.3239</v>
+      </c>
+      <c r="B9">
+        <v>2.69408</v>
+      </c>
+      <c r="C9">
+        <v>8.2892899999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>15.344900000000001</v>
+      </c>
+      <c r="B10">
+        <v>2.7053799999999999</v>
+      </c>
+      <c r="C10">
+        <v>8.5152400000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>15.3866</v>
+      </c>
+      <c r="B11">
+        <v>2.7191100000000001</v>
+      </c>
+      <c r="C11">
+        <v>8.2993500000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>15.4819</v>
+      </c>
+      <c r="B12">
+        <v>2.7098300000000002</v>
+      </c>
+      <c r="C12">
+        <v>8.4114900000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>15.4003</v>
+      </c>
+      <c r="B13">
+        <v>2.7833299999999999</v>
+      </c>
+      <c r="C13">
+        <v>8.12392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>15.337999999999999</v>
+      </c>
+      <c r="B14">
+        <v>2.9349400000000001</v>
+      </c>
+      <c r="C14">
+        <v>8.2017900000000008</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>15.416</v>
+      </c>
+      <c r="B15">
+        <v>2.8381099999999999</v>
+      </c>
+      <c r="C15">
+        <v>8.0960099999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15.345700000000001</v>
+      </c>
+      <c r="B16">
+        <v>2.8220000000000001</v>
+      </c>
+      <c r="C16">
+        <v>8.7003500000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618617AB-09A1-45C1-B83A-7FA81B820EEB}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>8.0154010000000007</v>
+      </c>
+      <c r="B2">
+        <v>2.10765</v>
+      </c>
+      <c r="C2">
+        <v>5.3207820000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>8.042783</v>
+      </c>
+      <c r="B3">
+        <v>2.0169790000000001</v>
+      </c>
+      <c r="C3">
+        <v>5.4305510000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>8.3339379999999998</v>
+      </c>
+      <c r="B4">
+        <v>2.0756839999999999</v>
+      </c>
+      <c r="C4">
+        <v>5.4702419999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8.1926140000000007</v>
+      </c>
+      <c r="B5">
+        <v>1.9903150000000001</v>
+      </c>
+      <c r="C5">
+        <v>5.2238049999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>7.9546559999999999</v>
+      </c>
+      <c r="B6">
+        <v>2.116606</v>
+      </c>
+      <c r="C6">
+        <v>5.6745869999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>8.0399759999999993</v>
+      </c>
+      <c r="B7">
+        <v>2.0226389999999999</v>
+      </c>
+      <c r="C7">
+        <v>5.0592199999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7.7916119999999998</v>
+      </c>
+      <c r="B8">
+        <v>2.1291920000000002</v>
+      </c>
+      <c r="C8">
+        <v>5.0897800000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8.0092370000000006</v>
+      </c>
+      <c r="B9">
+        <v>2.138217</v>
+      </c>
+      <c r="C9">
+        <v>5.1540499999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7.782089</v>
+      </c>
+      <c r="B10">
+        <v>2.0438200000000002</v>
+      </c>
+      <c r="C10">
+        <v>5.2308380000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>7.9253609999999997</v>
+      </c>
+      <c r="B11">
+        <v>2.0581179999999999</v>
+      </c>
+      <c r="C11">
+        <v>5.4985419999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>7.823359</v>
+      </c>
+      <c r="B12">
+        <v>2.1022120000000002</v>
+      </c>
+      <c r="C12">
+        <v>5.55267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7.8388530000000003</v>
+      </c>
+      <c r="B13">
+        <v>2.059307</v>
+      </c>
+      <c r="C13">
+        <v>4.3909609999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>7.7579700000000003</v>
+      </c>
+      <c r="B14">
+        <v>2.1428829999999999</v>
+      </c>
+      <c r="C14">
+        <v>5.4521490000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>7.8748050000000003</v>
+      </c>
+      <c r="B15">
+        <v>2.1609159999999998</v>
+      </c>
+      <c r="C15">
+        <v>5.4355909999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>7.8328800000000003</v>
+      </c>
+      <c r="B16">
+        <v>1.9799519999999999</v>
+      </c>
+      <c r="C16">
+        <v>5.0673890000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>